<commit_message>
arreglo discrepancias en datos de puntajes
</commit_message>
<xml_diff>
--- a/output/consolidated_data.xlsx
+++ b/output/consolidated_data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\rep_23\puntajes\output\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/664fb8667cea0a38/Documents/GitHub/puntajes_udea/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2152495-5A82-432E-8380-C033A6497665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{C2152495-5A82-432E-8380-C033A6497665}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{185FB986-85FE-462F-A481-3A2146D1F230}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24801,8 +24801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1171"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
-      <selection activeCell="C173" sqref="C173"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24879,7 +24879,7 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>3.496</v>
+        <v>3496</v>
       </c>
       <c r="D3">
         <v>87</v>
@@ -24931,7 +24931,7 @@
         <v>10</v>
       </c>
       <c r="C5">
-        <v>1.254</v>
+        <v>1254</v>
       </c>
       <c r="D5">
         <v>34</v>
@@ -25139,7 +25139,7 @@
         <v>10</v>
       </c>
       <c r="C13">
-        <v>1.077</v>
+        <v>1077</v>
       </c>
       <c r="D13">
         <v>49</v>
@@ -25165,7 +25165,7 @@
         <v>10</v>
       </c>
       <c r="C14">
-        <v>1.429</v>
+        <v>1429</v>
       </c>
       <c r="D14">
         <v>87</v>
@@ -25217,7 +25217,7 @@
         <v>10</v>
       </c>
       <c r="C16">
-        <v>1.341</v>
+        <v>1341</v>
       </c>
       <c r="D16">
         <v>21</v>
@@ -25243,7 +25243,7 @@
         <v>10</v>
       </c>
       <c r="C17">
-        <v>1.0429999999999999</v>
+        <v>1043</v>
       </c>
       <c r="D17">
         <v>30</v>
@@ -25269,7 +25269,7 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>2.04</v>
+        <v>204</v>
       </c>
       <c r="D18">
         <v>82</v>
@@ -25295,7 +25295,7 @@
         <v>32</v>
       </c>
       <c r="C19">
-        <v>1.177</v>
+        <v>1177</v>
       </c>
       <c r="D19">
         <v>53</v>
@@ -25321,7 +25321,7 @@
         <v>10</v>
       </c>
       <c r="C20">
-        <v>3.4239999999999999</v>
+        <v>3424</v>
       </c>
       <c r="D20">
         <v>137</v>
@@ -25399,7 +25399,7 @@
         <v>10</v>
       </c>
       <c r="C23">
-        <v>1.42</v>
+        <v>142</v>
       </c>
       <c r="D23">
         <v>92</v>
@@ -25425,7 +25425,7 @@
         <v>10</v>
       </c>
       <c r="C24">
-        <v>3.323</v>
+        <v>3323</v>
       </c>
       <c r="D24">
         <v>54</v>
@@ -25451,7 +25451,7 @@
         <v>10</v>
       </c>
       <c r="C25">
-        <v>1.655</v>
+        <v>1655</v>
       </c>
       <c r="D25">
         <v>41</v>
@@ -25919,7 +25919,7 @@
         <v>10</v>
       </c>
       <c r="C43">
-        <v>1.6639999999999999</v>
+        <v>1664</v>
       </c>
       <c r="D43">
         <v>80</v>
@@ -25997,7 +25997,7 @@
         <v>10</v>
       </c>
       <c r="C46">
-        <v>2.556</v>
+        <v>2556</v>
       </c>
       <c r="D46">
         <v>77</v>
@@ -26101,7 +26101,7 @@
         <v>10</v>
       </c>
       <c r="C50">
-        <v>2.2839999999999998</v>
+        <v>2284</v>
       </c>
       <c r="D50">
         <v>84</v>
@@ -26231,7 +26231,7 @@
         <v>10</v>
       </c>
       <c r="C55">
-        <v>1.0089999999999999</v>
+        <v>1009</v>
       </c>
       <c r="D55">
         <v>79</v>
@@ -26283,7 +26283,7 @@
         <v>10</v>
       </c>
       <c r="C57">
-        <v>1.6539999999999999</v>
+        <v>1654</v>
       </c>
       <c r="D57">
         <v>80</v>
@@ -26335,7 +26335,7 @@
         <v>10</v>
       </c>
       <c r="C59">
-        <v>1.4670000000000001</v>
+        <v>1467</v>
       </c>
       <c r="D59">
         <v>80</v>
@@ -26413,7 +26413,7 @@
         <v>10</v>
       </c>
       <c r="C62">
-        <v>2.085</v>
+        <v>2085</v>
       </c>
       <c r="D62">
         <v>36</v>
@@ -26462,7 +26462,7 @@
         <v>84</v>
       </c>
       <c r="C64">
-        <v>1.5289999999999999</v>
+        <v>1529</v>
       </c>
       <c r="D64">
         <v>40</v>
@@ -26592,7 +26592,7 @@
         <v>10</v>
       </c>
       <c r="C69">
-        <v>1.4430000000000001</v>
+        <v>1443</v>
       </c>
       <c r="D69">
         <v>67</v>
@@ -26800,7 +26800,7 @@
         <v>10</v>
       </c>
       <c r="C77">
-        <v>8.9380000000000006</v>
+        <v>8938</v>
       </c>
       <c r="D77">
         <v>137</v>
@@ -26826,7 +26826,7 @@
         <v>10</v>
       </c>
       <c r="C78">
-        <v>2.6960000000000002</v>
+        <v>2696</v>
       </c>
       <c r="D78">
         <v>59</v>
@@ -26904,7 +26904,7 @@
         <v>10</v>
       </c>
       <c r="C81">
-        <v>1.335</v>
+        <v>1335</v>
       </c>
       <c r="D81">
         <v>54</v>
@@ -26930,7 +26930,7 @@
         <v>10</v>
       </c>
       <c r="C82">
-        <v>2.2519999999999998</v>
+        <v>2252</v>
       </c>
       <c r="D82">
         <v>38</v>
@@ -27008,7 +27008,7 @@
         <v>10</v>
       </c>
       <c r="C85">
-        <v>2.1869999999999998</v>
+        <v>2187</v>
       </c>
       <c r="D85">
         <v>55</v>
@@ -27060,7 +27060,7 @@
         <v>10</v>
       </c>
       <c r="C87">
-        <v>1.1619999999999999</v>
+        <v>1162</v>
       </c>
       <c r="D87">
         <v>24</v>
@@ -27086,7 +27086,7 @@
         <v>10</v>
       </c>
       <c r="C88">
-        <v>3.6789999999999998</v>
+        <v>3679</v>
       </c>
       <c r="D88">
         <v>61</v>
@@ -27138,7 +27138,7 @@
         <v>32</v>
       </c>
       <c r="C90">
-        <v>1.1850000000000001</v>
+        <v>1185</v>
       </c>
       <c r="D90">
         <v>32</v>
@@ -27190,7 +27190,7 @@
         <v>10</v>
       </c>
       <c r="C92">
-        <v>1.046</v>
+        <v>1046</v>
       </c>
       <c r="D92">
         <v>46</v>
@@ -27216,7 +27216,7 @@
         <v>10</v>
       </c>
       <c r="C93">
-        <v>1.0289999999999999</v>
+        <v>1029</v>
       </c>
       <c r="D93">
         <v>61</v>
@@ -27762,7 +27762,7 @@
         <v>10</v>
       </c>
       <c r="C114">
-        <v>1.9970000000000001</v>
+        <v>1997</v>
       </c>
       <c r="D114">
         <v>58</v>
@@ -27840,7 +27840,7 @@
         <v>10</v>
       </c>
       <c r="C117">
-        <v>1.6830000000000001</v>
+        <v>1683</v>
       </c>
       <c r="D117">
         <v>41</v>
@@ -27866,7 +27866,7 @@
         <v>10</v>
       </c>
       <c r="C118">
-        <v>1.68</v>
+        <v>168</v>
       </c>
       <c r="D118">
         <v>57</v>
@@ -27918,7 +27918,7 @@
         <v>10</v>
       </c>
       <c r="C120">
-        <v>1.0880000000000001</v>
+        <v>1088</v>
       </c>
       <c r="D120">
         <v>87</v>
@@ -28334,7 +28334,7 @@
         <v>10</v>
       </c>
       <c r="C136">
-        <v>1.327</v>
+        <v>1327</v>
       </c>
       <c r="D136">
         <v>136</v>
@@ -28412,7 +28412,7 @@
         <v>10</v>
       </c>
       <c r="C139">
-        <v>1.6970000000000001</v>
+        <v>1697</v>
       </c>
       <c r="D139">
         <v>54</v>
@@ -29296,7 +29296,7 @@
         <v>10</v>
       </c>
       <c r="C173">
-        <v>1.2090000000000001</v>
+        <v>1209</v>
       </c>
       <c r="D173">
         <v>36</v>
@@ -29686,7 +29686,7 @@
         <v>10</v>
       </c>
       <c r="C188">
-        <v>4.5209999999999999</v>
+        <v>4521</v>
       </c>
       <c r="D188">
         <v>139</v>
@@ -29712,7 +29712,7 @@
         <v>10</v>
       </c>
       <c r="C189">
-        <v>1.359</v>
+        <v>1359</v>
       </c>
       <c r="D189">
         <v>53</v>
@@ -29816,7 +29816,7 @@
         <v>10</v>
       </c>
       <c r="C193">
-        <v>1.3069999999999999</v>
+        <v>1307</v>
       </c>
       <c r="D193">
         <v>29</v>
@@ -29842,7 +29842,7 @@
         <v>10</v>
       </c>
       <c r="C194">
-        <v>1.0149999999999999</v>
+        <v>1015</v>
       </c>
       <c r="D194">
         <v>55</v>
@@ -29920,7 +29920,7 @@
         <v>10</v>
       </c>
       <c r="C197">
-        <v>1.4179999999999999</v>
+        <v>1418</v>
       </c>
       <c r="D197">
         <v>58</v>

</xml_diff>